<commit_message>
Front-end connections and zoo! mock-up minor updates
</commit_message>
<xml_diff>
--- a/rom/Plans/Plans.xlsx
+++ b/rom/Plans/Plans.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Product ID</t>
   </si>
@@ -69,6 +69,73 @@
   </si>
   <si>
     <t>ksdajkadsjas</t>
+  </si>
+  <si>
+    <t>PL10</t>
+  </si>
+  <si>
+    <t>Camilo</t>
+  </si>
+  <si>
+    <t>dasads</t>
+  </si>
+  <si>
+    <t>PL11</t>
+  </si>
+  <si>
+    <t>Esteisi</t>
+  </si>
+  <si>
+    <t>dssdads</t>
+  </si>
+  <si>
+    <t>PL14</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>PL15</t>
+  </si>
+  <si>
+    <t>32312</t>
+  </si>
+  <si>
+    <t>PL16</t>
+  </si>
+  <si>
+    <t>Pangolines y Camacoles</t>
+  </si>
+  <si>
+    <t>¡Muy barato! Porque es sólo ir a ver a Pangolin
+en Camacol</t>
+  </si>
+  <si>
+    <t>PL17</t>
+  </si>
+  <si>
+    <t>¡Nuestro plan más barato! Te podrás divertir en Niquía Camacol para que conozcas a los Pangolines que frecuentan el Polideportivo y las extensas calles bellanitas</t>
+  </si>
+  <si>
+    <t>PL18</t>
+  </si>
+  <si>
+    <t>Pangolines</t>
+  </si>
+  <si>
+    <t>Usualmente nunca te encontrarás un pangolín en Colombia. Pero te encontrarás con la suerte de conocer uno en Camacol, por tan solo el valor de este plan te incluimos la visita al Polideportivo de Bello y la visita al mismísimo pangolín</t>
+  </si>
+  <si>
+    <t>PL19</t>
+  </si>
+  <si>
+    <t>Balazos</t>
+  </si>
+  <si>
+    <t>Este plan incluye un tour guiado por la Comuna 6 Bellavista de Bello, donde te adentrarás en la experiencia de esquivar balas, especialmente en el Barrio Pachelly.</t>
   </si>
 </sst>
 </file>
@@ -113,7 +180,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -135,72 +202,30 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C2" t="n">
-        <v>9.12813312E8</v>
+        <v>2250.0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>20200.0</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="n">
-        <v>231.0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3.12821907456E11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interfaz incluida y limpieza de comentarios
Ola
</commit_message>
<xml_diff>
--- a/rom/Plans/Plans.xlsx
+++ b/rom/Plans/Plans.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26407"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\Zoologico\rom\Plans\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Product ID</t>
   </si>
@@ -50,12 +50,22 @@
   </si>
   <si>
     <t>Este plan incluye un tour guiado por la Comuna 6 Bellavista de Bello, donde te adentrarás en la experiencia de esquivar balas, especialmente en el Barrio Pachelly.</t>
+  </si>
+  <si>
+    <t>PL20</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>asdasda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
@@ -451,6 +461,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="n">
+        <v>123123.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>